<commit_message>
Atualização de desafio com Excel
</commit_message>
<xml_diff>
--- a/planilhas/clientes.xlsx
+++ b/planilhas/clientes.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matheuspassossilva/Library/CloudStorage/Dropbox/GitHub/tratamento-arquivos/planilhas/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF5806C-A110-3842-BAA9-84FBEE605545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="34560" yWindow="-5960" windowWidth="51200" windowHeight="28300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS" sheetId="1" r:id="rId1"/>
@@ -1732,14 +1738,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-  </numFmts>
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -1747,346 +1747,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -2094,251 +1764,9 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2347,89 +1775,158 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Moeda" xfId="2" builtinId="4"/>
-    <cellStyle name="Porcentagem" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Moeda [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Hyperlink seguido" xfId="7" builtinId="9"/>
-    <cellStyle name="Observação" xfId="8" builtinId="10"/>
-    <cellStyle name="Texto de Aviso" xfId="9" builtinId="11"/>
-    <cellStyle name="Título" xfId="10" builtinId="15"/>
-    <cellStyle name="Texto Explicativo" xfId="11" builtinId="53"/>
-    <cellStyle name="Título 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Título 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Título 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Título 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Entrada" xfId="16" builtinId="20"/>
-    <cellStyle name="Saída" xfId="17" builtinId="21"/>
-    <cellStyle name="Cálculo" xfId="18" builtinId="22"/>
-    <cellStyle name="Célula de Verificação" xfId="19" builtinId="23"/>
-    <cellStyle name="Célula Vinculada" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Bom" xfId="22" builtinId="26"/>
-    <cellStyle name="Ruim" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutro" xfId="24" builtinId="28"/>
-    <cellStyle name="Ênfase 1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Ênfase 1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Ênfase 1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Ênfase 1" xfId="28" builtinId="32"/>
-    <cellStyle name="Ênfase 2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Ênfase 2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Ênfase 2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Ênfase 2" xfId="32" builtinId="36"/>
-    <cellStyle name="Ênfase 3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Ênfase 3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Ênfase 3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Ênfase 3" xfId="36" builtinId="40"/>
-    <cellStyle name="Ênfase 4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Ênfase 4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Ênfase 4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Ênfase 4" xfId="40" builtinId="44"/>
-    <cellStyle name="Ênfase 5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Ênfase 5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Ênfase 5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Ênfase 5" xfId="44" builtinId="48"/>
-    <cellStyle name="Ênfase 6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Ênfase 6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Ênfase 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Ênfase 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <color theme="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
         <color theme="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
         <color theme="1"/>
       </font>
       <border>
@@ -2440,7 +1937,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
         <color theme="0"/>
       </font>
       <fill>
@@ -2468,154 +1965,40 @@
           <color theme="4"/>
         </bottom>
         <horizontal style="thin">
-          <color theme="4" tint="0.399975585192419"/>
+          <color theme="4" tint="0.39994506668294322"/>
         </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <border>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
       </border>
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
     <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
-      <tableStyleElement type="wholeTable" dxfId="6"/>
-      <tableStyleElement type="headerRow" dxfId="5"/>
-      <tableStyleElement type="totalRow" dxfId="4"/>
-      <tableStyleElement type="firstColumn" dxfId="3"/>
-      <tableStyleElement type="lastColumn" dxfId="2"/>
-      <tableStyleElement type="firstRowStripe" dxfId="1"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="16"/>
+      <tableStyleElement type="headerRow" dxfId="15"/>
+      <tableStyleElement type="totalRow" dxfId="14"/>
+      <tableStyleElement type="firstColumn" dxfId="13"/>
+      <tableStyleElement type="lastColumn" dxfId="12"/>
+      <tableStyleElement type="firstRowStripe" dxfId="11"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="10"/>
     </tableStyle>
     <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
-      <tableStyleElement type="headerRow" dxfId="16"/>
-      <tableStyleElement type="totalRow" dxfId="15"/>
-      <tableStyleElement type="firstRowStripe" dxfId="14"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="8"/>
-      <tableStyleElement type="pageFieldValues" dxfId="7"/>
+      <tableStyleElement type="headerRow" dxfId="9"/>
+      <tableStyleElement type="totalRow" dxfId="8"/>
+      <tableStyleElement type="firstRowStripe" dxfId="7"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="6"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="5"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="4"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="3"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="2"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="1"/>
+      <tableStyleElement type="pageFieldValues" dxfId="0"/>
     </tableStyle>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2873,25 +2256,23 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52:D63"/>
-    </sheetView>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="16.8571428571429" customWidth="1"/>
+    <col min="1" max="1" width="20.796875" customWidth="1"/>
+    <col min="2" max="2" width="16.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2905,7 +2286,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2919,7 +2300,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2933,7 +2314,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2947,7 +2328,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -2961,7 +2342,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -2975,7 +2356,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2989,7 +2370,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -3003,7 +2384,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -3017,7 +2398,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -3031,7 +2412,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -3045,7 +2426,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -3059,7 +2440,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -3073,7 +2454,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -3087,7 +2468,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -3101,7 +2482,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -3115,7 +2496,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -3129,7 +2510,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -3143,7 +2524,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -3157,7 +2538,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -3171,7 +2552,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -3185,7 +2566,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -3199,7 +2580,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -3213,7 +2594,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>70</v>
       </c>
@@ -3227,7 +2608,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>73</v>
       </c>
@@ -3241,7 +2622,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>76</v>
       </c>
@@ -3255,7 +2636,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>79</v>
       </c>
@@ -3269,7 +2650,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>82</v>
       </c>
@@ -3283,7 +2664,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>85</v>
       </c>
@@ -3297,7 +2678,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>88</v>
       </c>
@@ -3311,7 +2692,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>91</v>
       </c>
@@ -3325,7 +2706,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -3339,7 +2720,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -3353,7 +2734,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>100</v>
       </c>
@@ -3367,7 +2748,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>103</v>
       </c>
@@ -3381,7 +2762,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>106</v>
       </c>
@@ -3395,7 +2776,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>109</v>
       </c>
@@ -3409,7 +2790,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>112</v>
       </c>
@@ -3423,7 +2804,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>115</v>
       </c>
@@ -3437,7 +2818,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>118</v>
       </c>
@@ -3451,7 +2832,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>121</v>
       </c>
@@ -3465,7 +2846,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>124</v>
       </c>
@@ -3479,7 +2860,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>127</v>
       </c>
@@ -3493,7 +2874,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>130</v>
       </c>
@@ -3507,7 +2888,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>133</v>
       </c>
@@ -3521,7 +2902,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>136</v>
       </c>
@@ -3535,7 +2916,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>139</v>
       </c>
@@ -3549,7 +2930,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>142</v>
       </c>
@@ -3563,7 +2944,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>145</v>
       </c>
@@ -3577,7 +2958,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>148</v>
       </c>
@@ -3591,7 +2972,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>151</v>
       </c>
@@ -3607,22 +2988,24 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37:D63"/>
-    </sheetView>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3636,7 +3019,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>154</v>
       </c>
@@ -3650,7 +3033,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>157</v>
       </c>
@@ -3664,7 +3047,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>160</v>
       </c>
@@ -3678,7 +3061,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>163</v>
       </c>
@@ -3692,7 +3075,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>166</v>
       </c>
@@ -3706,7 +3089,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>169</v>
       </c>
@@ -3720,7 +3103,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>172</v>
       </c>
@@ -3734,7 +3117,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>175</v>
       </c>
@@ -3748,7 +3131,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>178</v>
       </c>
@@ -3762,7 +3145,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>181</v>
       </c>
@@ -3776,7 +3159,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>184</v>
       </c>
@@ -3790,7 +3173,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>187</v>
       </c>
@@ -3804,7 +3187,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>190</v>
       </c>
@@ -3818,7 +3201,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>193</v>
       </c>
@@ -3832,7 +3215,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>196</v>
       </c>
@@ -3846,7 +3229,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>199</v>
       </c>
@@ -3860,7 +3243,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>202</v>
       </c>
@@ -3874,7 +3257,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>205</v>
       </c>
@@ -3888,7 +3271,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>208</v>
       </c>
@@ -3902,7 +3285,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>211</v>
       </c>
@@ -3916,7 +3299,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>214</v>
       </c>
@@ -3930,7 +3313,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>217</v>
       </c>
@@ -3944,7 +3327,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>220</v>
       </c>
@@ -3958,7 +3341,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>223</v>
       </c>
@@ -3972,7 +3355,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>226</v>
       </c>
@@ -3986,7 +3369,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>229</v>
       </c>
@@ -4000,7 +3383,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>232</v>
       </c>
@@ -4014,7 +3397,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>235</v>
       </c>
@@ -4028,7 +3411,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>238</v>
       </c>
@@ -4042,7 +3425,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>241</v>
       </c>
@@ -4056,7 +3439,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>244</v>
       </c>
@@ -4070,7 +3453,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>247</v>
       </c>
@@ -4084,7 +3467,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>250</v>
       </c>
@@ -4098,7 +3481,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>253</v>
       </c>
@@ -4112,7 +3495,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>256</v>
       </c>
@@ -4128,22 +3511,24 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
-    </sheetView>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4157,7 +3542,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>259</v>
       </c>
@@ -4171,7 +3556,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>262</v>
       </c>
@@ -4185,7 +3570,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>265</v>
       </c>
@@ -4199,7 +3584,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>268</v>
       </c>
@@ -4213,7 +3598,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>271</v>
       </c>
@@ -4227,7 +3612,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>274</v>
       </c>
@@ -4241,7 +3626,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>277</v>
       </c>
@@ -4255,7 +3640,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>280</v>
       </c>
@@ -4269,7 +3654,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>283</v>
       </c>
@@ -4283,7 +3668,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>286</v>
       </c>
@@ -4297,7 +3682,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>289</v>
       </c>
@@ -4311,7 +3696,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>292</v>
       </c>
@@ -4325,7 +3710,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>295</v>
       </c>
@@ -4339,7 +3724,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>298</v>
       </c>
@@ -4353,7 +3738,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>301</v>
       </c>
@@ -4367,7 +3752,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>304</v>
       </c>
@@ -4381,7 +3766,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>307</v>
       </c>
@@ -4395,7 +3780,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>310</v>
       </c>
@@ -4409,7 +3794,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>313</v>
       </c>
@@ -4423,7 +3808,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>316</v>
       </c>
@@ -4437,7 +3822,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>319</v>
       </c>
@@ -4451,7 +3836,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>322</v>
       </c>
@@ -4465,7 +3850,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>325</v>
       </c>
@@ -4479,7 +3864,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>328</v>
       </c>
@@ -4493,7 +3878,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>331</v>
       </c>
@@ -4507,7 +3892,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>334</v>
       </c>
@@ -4521,7 +3906,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>337</v>
       </c>
@@ -4535,7 +3920,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>340</v>
       </c>
@@ -4549,7 +3934,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>343</v>
       </c>
@@ -4563,7 +3948,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>346</v>
       </c>
@@ -4577,7 +3962,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>349</v>
       </c>
@@ -4591,7 +3976,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>352</v>
       </c>
@@ -4605,7 +3990,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>355</v>
       </c>
@@ -4619,7 +4004,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>358</v>
       </c>
@@ -4633,7 +4018,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>361</v>
       </c>
@@ -4647,7 +4032,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>364</v>
       </c>
@@ -4661,7 +4046,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>367</v>
       </c>
@@ -4675,7 +4060,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>370</v>
       </c>
@@ -4689,7 +4074,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>373</v>
       </c>
@@ -4703,7 +4088,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>376</v>
       </c>
@@ -4717,7 +4102,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>379</v>
       </c>
@@ -4731,7 +4116,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>382</v>
       </c>
@@ -4747,22 +4132,24 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4776,7 +4163,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>385</v>
       </c>
@@ -4790,7 +4177,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>388</v>
       </c>
@@ -4804,7 +4191,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>391</v>
       </c>
@@ -4818,7 +4205,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>394</v>
       </c>
@@ -4832,7 +4219,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>397</v>
       </c>
@@ -4846,7 +4233,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>400</v>
       </c>
@@ -4860,7 +4247,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>403</v>
       </c>
@@ -4874,7 +4261,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>406</v>
       </c>
@@ -4888,7 +4275,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>409</v>
       </c>
@@ -4902,7 +4289,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>412</v>
       </c>
@@ -4916,7 +4303,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>415</v>
       </c>
@@ -4930,7 +4317,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>418</v>
       </c>
@@ -4944,7 +4331,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>421</v>
       </c>
@@ -4958,7 +4345,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>424</v>
       </c>
@@ -4972,7 +4359,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>427</v>
       </c>
@@ -4986,7 +4373,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>430</v>
       </c>
@@ -5000,7 +4387,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>433</v>
       </c>
@@ -5014,7 +4401,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>436</v>
       </c>
@@ -5028,7 +4415,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>439</v>
       </c>
@@ -5042,7 +4429,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>442</v>
       </c>
@@ -5056,7 +4443,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>445</v>
       </c>
@@ -5070,7 +4457,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>448</v>
       </c>
@@ -5084,7 +4471,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>451</v>
       </c>
@@ -5098,7 +4485,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>454</v>
       </c>
@@ -5112,7 +4499,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>457</v>
       </c>
@@ -5126,7 +4513,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>460</v>
       </c>
@@ -5140,7 +4527,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>463</v>
       </c>
@@ -5154,7 +4541,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>466</v>
       </c>
@@ -5168,7 +4555,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>469</v>
       </c>
@@ -5182,7 +4569,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>472</v>
       </c>
@@ -5196,7 +4583,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>475</v>
       </c>
@@ -5210,7 +4597,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>478</v>
       </c>
@@ -5224,7 +4611,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>481</v>
       </c>
@@ -5238,7 +4625,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>484</v>
       </c>
@@ -5252,7 +4639,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>487</v>
       </c>
@@ -5266,7 +4653,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>490</v>
       </c>
@@ -5280,7 +4667,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>493</v>
       </c>
@@ -5294,7 +4681,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>496</v>
       </c>
@@ -5308,7 +4695,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>499</v>
       </c>
@@ -5322,7 +4709,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>502</v>
       </c>
@@ -5336,7 +4723,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>505</v>
       </c>
@@ -5350,7 +4737,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>508</v>
       </c>
@@ -5364,7 +4751,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>511</v>
       </c>
@@ -5378,7 +4765,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>514</v>
       </c>
@@ -5392,7 +4779,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>516</v>
       </c>
@@ -5406,7 +4793,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>519</v>
       </c>
@@ -5420,7 +4807,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>522</v>
       </c>
@@ -5434,7 +4821,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>525</v>
       </c>
@@ -5448,7 +4835,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>528</v>
       </c>
@@ -5462,7 +4849,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>531</v>
       </c>
@@ -5476,7 +4863,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>534</v>
       </c>
@@ -5490,7 +4877,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>537</v>
       </c>
@@ -5504,7 +4891,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>540</v>
       </c>
@@ -5518,7 +4905,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>543</v>
       </c>
@@ -5532,7 +4919,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>546</v>
       </c>
@@ -5546,7 +4933,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>549</v>
       </c>
@@ -5560,7 +4947,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>552</v>
       </c>
@@ -5574,7 +4961,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>555</v>
       </c>
@@ -5588,7 +4975,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>558</v>
       </c>
@@ -5602,7 +4989,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>561</v>
       </c>
@@ -5616,7 +5003,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>564</v>
       </c>
@@ -5630,7 +5017,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>567</v>
       </c>
@@ -5646,6 +5033,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>